<commit_message>
presentación división, 2 de 4 graf, top dflt =15, comentada fncn compleja
</commit_message>
<xml_diff>
--- a/datosAdicionales.xlsx
+++ b/datosAdicionales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dccpcompras-my.sharepoint.com/personal/diego_martinez_chilecompra_cl/Documents/Escritorio/Dpt Comunicaciones/Reportes Automatizados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="11_AD4D2F04E46CFB4ACB3E20E085D3E622683EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{941FD659-E79F-4AE5-A49E-652495726807}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="11_AD4D2F04E46CFB4ACB3E20E085D3E622683EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AAF94D0-F0A0-47E1-8990-19860E8763D4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -445,7 +445,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>